<commit_message>
various adjusts to the system
</commit_message>
<xml_diff>
--- a/cupom.xlsx
+++ b/cupom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao.vitor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.augusto\Desktop\trade_sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6176D9A7-705D-4817-925E-8F15501EAC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622C7FFF-11C5-4CFF-B176-07FCC19CBE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>CUPOM DE VENDA</t>
   </si>
@@ -43,15 +43,6 @@
   </si>
   <si>
     <t>PAO DE SAL KG</t>
-  </si>
-  <si>
-    <t>ESSE CUPOM PERDE A VALIDADE</t>
-  </si>
-  <si>
-    <t>APOS A VENDA, PASSADO O PRAZO</t>
-  </si>
-  <si>
-    <t>CUPOM VALIDO POR 3 DIAS</t>
   </si>
 </sst>
 </file>
@@ -379,7 +370,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,21 +383,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>

</xml_diff>